<commit_message>
with this tracker two we can send bulk mails without problem and multiple attachments at time
</commit_message>
<xml_diff>
--- a/reclog.xlsx
+++ b/reclog.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,210 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>rec1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cnumani@outlook.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rec2</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>reddy.binary@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rec3</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>indumathilalam03@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rec1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>cnumani@outlook.com</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rec2</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>reddy.binary@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>rec3</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>indumathilalam03@gmail.com</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>rec1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>cnumani@outlook.com</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>rec2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>reddy.binary@gmail.com</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>rec3</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>indumathilalam03@gmail.com</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>cnumani</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>cnumani@outlook.com</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>binary</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>reddy.binary@gmail.com</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>indumanthi</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>indumathilalam03@gmail.com</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2024-10-17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>